<commit_message>
final page. fully functional and ready to play!
</commit_message>
<xml_diff>
--- a/images/product info.xlsx
+++ b/images/product info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="2860" windowWidth="13700" windowHeight="12640" tabRatio="500"/>
+    <workbookView xWindow="22920" yWindow="0" windowWidth="13700" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>image link</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Product title</t>
   </si>
@@ -46,13 +43,115 @@
   </si>
   <si>
     <t>Brooks England B17 Special Saddle</t>
+  </si>
+  <si>
+    <t>Breville BES860XL Espresso Machine with Grinder</t>
+  </si>
+  <si>
+    <t>Ninja Mega Kitchen System</t>
+  </si>
+  <si>
+    <t>KitchenAid 11-Cup Food Processor with Exact Slice System</t>
+  </si>
+  <si>
+    <t>George Foreman GGR50B Indoor/Outdoor Grill</t>
+  </si>
+  <si>
+    <t>Zojirushi NS-TSC10 5.5-Cup Micom Rice Cooker and Warmer</t>
+  </si>
+  <si>
+    <t>GinsuChikara 8-Piece Stainless Steel Knife Set with Bamboo Block</t>
+  </si>
+  <si>
+    <t>Gibson Elite Tequesta 16-Piece Square Dinnerware Set</t>
+  </si>
+  <si>
+    <t>Transition Scout 2Full Suspension Mountain Bike</t>
+  </si>
+  <si>
+    <t>Electric FW02 Nato Watch</t>
+  </si>
+  <si>
+    <t>Nixon The Time Teller Acetate Watch</t>
+  </si>
+  <si>
+    <t>Chrome Barrage Backpack</t>
+  </si>
+  <si>
+    <t>Red Wing 8138 6-Inch Moc Boots</t>
+  </si>
+  <si>
+    <t>Eames Lounge Chair</t>
+  </si>
+  <si>
+    <t>XCEL 4/3mm Infiniti X2 Hooded Wetsuit</t>
+  </si>
+  <si>
+    <t>Poler Napsack</t>
+  </si>
+  <si>
+    <t>Skullcandy Air Raid Bluetooth Speakers</t>
+  </si>
+  <si>
+    <t>Smith Forefront Bike Helmet</t>
+  </si>
+  <si>
+    <t>GoPro Hero4 Black Camera</t>
+  </si>
+  <si>
+    <t>Fitbit Surge Fitness Superwatch</t>
+  </si>
+  <si>
+    <t>Sony 4K 3D Blu-ray Disc Player With Dual Core Processor</t>
+  </si>
+  <si>
+    <t>Samsung UN65JS8500 65-Inch 4K Ultra HD Smart LED TV</t>
+  </si>
+  <si>
+    <t>Bose CineMate 520 Home Theater System</t>
+  </si>
+  <si>
+    <t>Callaway Men's Strata Ultimate Complete Golf Set</t>
+  </si>
+  <si>
+    <t>STIGA InstaPlay Table Tennis Table</t>
+  </si>
+  <si>
+    <t>Precor 211 Energy Series Treadmill</t>
+  </si>
+  <si>
+    <t>Xbox One, 500GB Hard Drive</t>
+  </si>
+  <si>
+    <t>Apple iPad Air 2 128GB/Wi-Fi</t>
+  </si>
+  <si>
+    <t>Garmin Edge 1000 Color Touchscreen GPS</t>
+  </si>
+  <si>
+    <t>DeWalt 20-Volt Lithium-Ion Cordless Brushless Compact Drill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Echo 18 in. 40.2 cc Gas Chainsaw</t>
+  </si>
+  <si>
+    <t>Hampton Bay Fall River 7-Piece Patio Dining Set</t>
+  </si>
+  <si>
+    <t>Raleigh Record Ace</t>
+  </si>
+  <si>
+    <t>BCA Tracker DTS Rescue Package 2015</t>
+  </si>
+  <si>
+    <t>Sorel Joan of Arctic Wedge Mid Boots</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,13 +183,32 @@
       <color rgb="FF111111"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,22 +220,308 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="143">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -448,82 +852,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C9"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A21" sqref="A21:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="3" t="s">
+      <c r="B2" s="4">
+        <v>399.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="32">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>399.99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="32">
-      <c r="B5" s="4" t="s">
+      <c r="B3" s="4">
+        <v>599.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="B4" s="4">
+        <v>69.989999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7">
+        <v>39.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7">
+        <v>53.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7">
+        <v>799.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7">
+        <v>219.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7">
+        <v>249.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7">
+        <v>199.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>149.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>79.989999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <v>199.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
+        <v>3929</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>359.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
+        <v>129.94999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4">
+        <v>149.94999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
+        <v>219.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4">
+        <v>499.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4">
+        <v>249.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4">
+        <v>299.99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4">
+        <v>699.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="4">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4">
         <v>599.99</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>69.989999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15">
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5">
-        <v>39.99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15">
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5">
-        <v>53.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15">
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5">
-        <v>171</v>
+    <row r="36" spans="1:2">
+      <c r="A36" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="4">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="4">
+        <v>319.95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="4">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2" display="AmazonBasics 8-Sheet High-Security"/>
-    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2" display="AmazonBasics 8-Sheet High-Security"/>
+    <hyperlink ref="A7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>